<commit_message>
fixed compound attrs; removed attribs
</commit_message>
<xml_diff>
--- a/dist/rd3_overview.xlsx
+++ b/dist/rd3_overview.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="146">
   <si>
     <t>rd3</t>
   </si>
@@ -49,9 +49,6 @@
     <t>genderAtBirth</t>
   </si>
   <si>
-    <t>yearOfBirth</t>
-  </si>
-  <si>
     <t>belongsToFamily</t>
   </si>
   <si>
@@ -172,9 +169,6 @@
     <t>Assigned gender is one's gender which was assigned at birth, typically by a medical and/or legal organization, and then later registered with other organizations. Such a designation is typically based off of the superficial appearance of external genitalia present at birth.</t>
   </si>
   <si>
-    <t>The year in which this person was born.</t>
-  </si>
-  <si>
     <t>A domestic group, or a number of domestic groups linked through descent (demonstrated or stipulated) from a common ancestor, marriage, or adoption.</t>
   </si>
   <si>
@@ -214,9 +208,6 @@
     <t>http://purl.obolibrary.org/obo/GSSO_009418</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C83164</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C25173</t>
   </si>
   <si>
@@ -247,18 +238,18 @@
     <t>xref</t>
   </si>
   <si>
+    <t>mref</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>compound</t>
+  </si>
+  <si>
     <t>int</t>
   </si>
   <si>
-    <t>mref</t>
-  </si>
-  <si>
-    <t>bool</t>
-  </si>
-  <si>
-    <t>compound</t>
-  </si>
-  <si>
     <t>rd3_sex</t>
   </si>
   <si>
@@ -376,6 +367,9 @@
     <t>refEntity</t>
   </si>
   <si>
+    <t>partOfAttribute</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/ExO_0000127</t>
   </si>
   <si>
@@ -419,9 +413,6 @@
   </si>
   <si>
     <t>NCIT:C80271</t>
-  </si>
-  <si>
-    <t>NCIT:C83164</t>
   </si>
   <si>
     <t>NCIT:C89336</t>
@@ -831,13 +822,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -866,19 +857,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -908,45 +899,48 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -954,13 +948,13 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -975,7 +969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -983,13 +977,13 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -1004,10 +998,10 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1015,13 +1009,13 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -1036,7 +1030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1044,13 +1038,13 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -1064,8 +1058,11 @@
       <c r="I5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="J5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1073,13 +1070,13 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -1097,7 +1094,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1105,13 +1102,13 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -1126,10 +1123,10 @@
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1137,13 +1134,10 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -1158,10 +1152,10 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1169,10 +1163,13 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -1187,10 +1184,10 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1198,13 +1195,13 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -1218,11 +1215,8 @@
       <c r="I10" t="b">
         <v>0</v>
       </c>
-      <c r="J10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1230,13 +1224,10 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -1251,7 +1242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1259,10 +1250,13 @@
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
@@ -1276,8 +1270,11 @@
       <c r="I12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="J12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1285,13 +1282,13 @@
         <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -1306,10 +1303,10 @@
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1317,13 +1314,13 @@
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E14" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -1338,24 +1335,18 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>7</v>
       </c>
       <c r="B15" t="s">
         <v>21</v>
       </c>
-      <c r="C15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="E15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -1369,11 +1360,8 @@
       <c r="I15" t="b">
         <v>0</v>
       </c>
-      <c r="J15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1381,7 +1369,7 @@
         <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -1395,8 +1383,11 @@
       <c r="I16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1404,7 +1395,7 @@
         <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
@@ -1418,8 +1409,14 @@
       <c r="I17" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="J17" t="s">
+        <v>83</v>
+      </c>
+      <c r="K17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1427,7 +1424,7 @@
         <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
@@ -1442,10 +1439,13 @@
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <v>84</v>
+      </c>
+      <c r="K18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -1468,10 +1468,13 @@
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+        <v>85</v>
+      </c>
+      <c r="K19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1479,7 +1482,7 @@
         <v>26</v>
       </c>
       <c r="E20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
@@ -1494,10 +1497,13 @@
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+        <v>86</v>
+      </c>
+      <c r="K20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1505,7 +1511,7 @@
         <v>27</v>
       </c>
       <c r="E21" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
@@ -1520,10 +1526,13 @@
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+        <v>87</v>
+      </c>
+      <c r="K21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1531,7 +1540,7 @@
         <v>28</v>
       </c>
       <c r="E22" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
@@ -1546,10 +1555,13 @@
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+        <v>88</v>
+      </c>
+      <c r="K22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1557,7 +1569,7 @@
         <v>29</v>
       </c>
       <c r="E23" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -1572,10 +1584,13 @@
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+        <v>89</v>
+      </c>
+      <c r="K23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1583,7 +1598,7 @@
         <v>30</v>
       </c>
       <c r="E24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
@@ -1597,11 +1612,8 @@
       <c r="I24" t="b">
         <v>0</v>
       </c>
-      <c r="J24" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -1609,7 +1621,7 @@
         <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
@@ -1623,8 +1635,11 @@
       <c r="I25" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="K25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1632,7 +1647,7 @@
         <v>32</v>
       </c>
       <c r="E26" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
@@ -1646,8 +1661,14 @@
       <c r="I26" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="J26" t="s">
+        <v>90</v>
+      </c>
+      <c r="K26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1655,7 +1676,7 @@
         <v>33</v>
       </c>
       <c r="E27" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
@@ -1670,10 +1691,13 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+        <v>91</v>
+      </c>
+      <c r="K27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1681,7 +1705,7 @@
         <v>34</v>
       </c>
       <c r="E28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F28" t="b">
         <v>0</v>
@@ -1696,10 +1720,13 @@
         <v>0</v>
       </c>
       <c r="J28" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
+        <v>92</v>
+      </c>
+      <c r="K28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1707,7 +1734,7 @@
         <v>35</v>
       </c>
       <c r="E29" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F29" t="b">
         <v>0</v>
@@ -1722,10 +1749,13 @@
         <v>0</v>
       </c>
       <c r="J29" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+        <v>93</v>
+      </c>
+      <c r="K29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -1733,7 +1763,7 @@
         <v>36</v>
       </c>
       <c r="E30" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F30" t="b">
         <v>0</v>
@@ -1748,10 +1778,13 @@
         <v>0</v>
       </c>
       <c r="J30" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
+        <v>94</v>
+      </c>
+      <c r="K30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1759,7 +1792,7 @@
         <v>37</v>
       </c>
       <c r="E31" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
@@ -1774,10 +1807,13 @@
         <v>0</v>
       </c>
       <c r="J31" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
+        <v>95</v>
+      </c>
+      <c r="K31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1785,7 +1821,7 @@
         <v>38</v>
       </c>
       <c r="E32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F32" t="b">
         <v>0</v>
@@ -1800,10 +1836,13 @@
         <v>0</v>
       </c>
       <c r="J32" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
+        <v>96</v>
+      </c>
+      <c r="K32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -1811,7 +1850,7 @@
         <v>39</v>
       </c>
       <c r="E33" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F33" t="b">
         <v>0</v>
@@ -1825,11 +1864,8 @@
       <c r="I33" t="b">
         <v>0</v>
       </c>
-      <c r="J33" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -1837,7 +1873,7 @@
         <v>40</v>
       </c>
       <c r="E34" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
@@ -1851,8 +1887,11 @@
       <c r="I34" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="K34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -1860,7 +1899,7 @@
         <v>41</v>
       </c>
       <c r="E35" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
@@ -1874,8 +1913,14 @@
       <c r="I35" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="J35" t="s">
+        <v>97</v>
+      </c>
+      <c r="K35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -1883,7 +1928,7 @@
         <v>42</v>
       </c>
       <c r="E36" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
@@ -1898,10 +1943,13 @@
         <v>0</v>
       </c>
       <c r="J36" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
+        <v>98</v>
+      </c>
+      <c r="K36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1909,7 +1957,7 @@
         <v>43</v>
       </c>
       <c r="E37" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F37" t="b">
         <v>0</v>
@@ -1924,10 +1972,13 @@
         <v>0</v>
       </c>
       <c r="J37" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
+        <v>99</v>
+      </c>
+      <c r="K37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -1935,7 +1986,7 @@
         <v>44</v>
       </c>
       <c r="E38" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F38" t="b">
         <v>0</v>
@@ -1950,10 +2001,13 @@
         <v>0</v>
       </c>
       <c r="J38" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
+        <v>100</v>
+      </c>
+      <c r="K38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1961,7 +2015,7 @@
         <v>45</v>
       </c>
       <c r="E39" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
@@ -1976,10 +2030,13 @@
         <v>0</v>
       </c>
       <c r="J39" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
+        <v>101</v>
+      </c>
+      <c r="K39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -1987,7 +2044,7 @@
         <v>46</v>
       </c>
       <c r="E40" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F40" t="b">
         <v>0</v>
@@ -2002,10 +2059,13 @@
         <v>0</v>
       </c>
       <c r="J40" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
+        <v>102</v>
+      </c>
+      <c r="K40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -2013,7 +2073,7 @@
         <v>47</v>
       </c>
       <c r="E41" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F41" t="b">
         <v>0</v>
@@ -2028,33 +2088,10 @@
         <v>0</v>
       </c>
       <c r="J41" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
-      <c r="A42" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" t="s">
-        <v>48</v>
-      </c>
-      <c r="E42" t="s">
-        <v>77</v>
-      </c>
-      <c r="F42" t="b">
-        <v>0</v>
-      </c>
-      <c r="G42" t="b">
-        <v>0</v>
-      </c>
-      <c r="H42" t="b">
-        <v>1</v>
-      </c>
-      <c r="I42" t="b">
-        <v>0</v>
-      </c>
-      <c r="J42" t="s">
-        <v>106</v>
+        <v>103</v>
+      </c>
+      <c r="K41" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2065,12 +2102,11 @@
     <hyperlink ref="D5" r:id="rId4"/>
     <hyperlink ref="D6" r:id="rId5"/>
     <hyperlink ref="D7" r:id="rId6"/>
-    <hyperlink ref="D8" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId7"/>
     <hyperlink ref="D10" r:id="rId8"/>
-    <hyperlink ref="D11" r:id="rId9"/>
+    <hyperlink ref="D12" r:id="rId9"/>
     <hyperlink ref="D13" r:id="rId10"/>
     <hyperlink ref="D14" r:id="rId11"/>
-    <hyperlink ref="D15" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2078,7 +2114,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2086,302 +2122,282 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" t="s">
         <v>139</v>
       </c>
-      <c r="E4" t="s">
-        <v>142</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="E5" t="s">
-        <v>142</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="E6" t="s">
-        <v>142</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D7" t="s">
+        <v>137</v>
+      </c>
+      <c r="E7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="E7" t="s">
-        <v>142</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="E8" t="s">
-        <v>142</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D9" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="E9" t="s">
-        <v>142</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" t="s">
+        <v>139</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="E10" t="s">
-        <v>142</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D11" t="s">
+        <v>137</v>
+      </c>
+      <c r="E11" t="s">
+        <v>139</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="E11" t="s">
-        <v>142</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="E12" t="s">
-        <v>142</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="E13" t="s">
-        <v>142</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
+        <v>138</v>
+      </c>
+      <c r="E14" t="s">
+        <v>139</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="E14" t="s">
-        <v>142</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" t="s">
-        <v>136</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" t="s">
-        <v>141</v>
-      </c>
-      <c r="E15" t="s">
-        <v>142</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2425,9 +2441,6 @@
     <hyperlink ref="A14" r:id="rId37"/>
     <hyperlink ref="C14" r:id="rId38"/>
     <hyperlink ref="F14" r:id="rId39" location="isAssociatedWith"/>
-    <hyperlink ref="A15" r:id="rId40"/>
-    <hyperlink ref="C15" r:id="rId41"/>
-    <hyperlink ref="F15" r:id="rId42" location="isAssociatedWith"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
aligned attribute names with rd3; added labels; rebuilt
</commit_message>
<xml_diff>
--- a/dist/rd3_overview.xlsx
+++ b/dist/rd3_overview.xlsx
@@ -10,14 +10,13 @@
     <sheet name="packages" sheetId="1" r:id="rId1"/>
     <sheet name="entities" sheetId="2" r:id="rId2"/>
     <sheet name="attributes" sheetId="3" r:id="rId3"/>
-    <sheet name="tags" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="146">
   <si>
     <t>rd3</t>
   </si>
@@ -46,43 +45,40 @@
     <t>subjectID</t>
   </si>
   <si>
-    <t>genderAtBirth</t>
-  </si>
-  <si>
-    <t>belongsToFamily</t>
-  </si>
-  <si>
-    <t>belongsToMother</t>
-  </si>
-  <si>
-    <t>belongsToFather</t>
-  </si>
-  <si>
-    <t>partOfDataRelease</t>
-  </si>
-  <si>
-    <t>primaryAffiliatedInstitute</t>
-  </si>
-  <si>
-    <t>participatesInStudy</t>
+    <t>sex1</t>
+  </si>
+  <si>
+    <t>fid</t>
+  </si>
+  <si>
+    <t>mid</t>
+  </si>
+  <si>
+    <t>pid</t>
+  </si>
+  <si>
+    <t>patch</t>
+  </si>
+  <si>
+    <t>organisation</t>
+  </si>
+  <si>
+    <t>ERN</t>
   </si>
   <si>
     <t>affectedStatus</t>
   </si>
   <si>
-    <t>solvedStatus</t>
-  </si>
-  <si>
-    <t>observedPhenotype</t>
-  </si>
-  <si>
-    <t>unobservedPhenotype</t>
-  </si>
-  <si>
-    <t>clinicalDiagnosis</t>
-  </si>
-  <si>
-    <t>emxRelease</t>
+    <t>solved</t>
+  </si>
+  <si>
+    <t>phenotype</t>
+  </si>
+  <si>
+    <t>hasNotPhenotype</t>
+  </si>
+  <si>
+    <t>disease</t>
   </si>
   <si>
     <t>samples</t>
@@ -106,6 +102,9 @@
     <t>novelrnaseqSamples</t>
   </si>
   <si>
+    <t>novellrwgsSamples</t>
+  </si>
+  <si>
     <t>novelsrwgsSamples</t>
   </si>
   <si>
@@ -166,6 +165,9 @@
     <t>novelwgsFile</t>
   </si>
   <si>
+    <t>associatedRD3Releases</t>
+  </si>
+  <si>
     <t>A unique proper name or character sequence that identifies this particular individual who is the subject of personal data, persons to whom data refers, and from whom data are collected, processed, and stored.</t>
   </si>
   <si>
@@ -259,6 +261,99 @@
     <t>hyperlink</t>
   </si>
   <si>
+    <t>Claimed Sex</t>
+  </si>
+  <si>
+    <t>FamilyID</t>
+  </si>
+  <si>
+    <t>MaternalID</t>
+  </si>
+  <si>
+    <t>PaternalID</t>
+  </si>
+  <si>
+    <t>Patch</t>
+  </si>
+  <si>
+    <t>Organisation</t>
+  </si>
+  <si>
+    <t>Affected Status</t>
+  </si>
+  <si>
+    <t>Total Number of Samples</t>
+  </si>
+  <si>
+    <t>DF1 Samples</t>
+  </si>
+  <si>
+    <t>DF2 Samples</t>
+  </si>
+  <si>
+    <t>DF3 Samples</t>
+  </si>
+  <si>
+    <t>NovelOmics Deep-WES Samples</t>
+  </si>
+  <si>
+    <t>NovelOmics RNAseq Samples</t>
+  </si>
+  <si>
+    <t>NovelOmics LR-WGS Samples</t>
+  </si>
+  <si>
+    <t>NovelOmics SR-WGS Samples</t>
+  </si>
+  <si>
+    <t>NovelOmics WGS Samples</t>
+  </si>
+  <si>
+    <t>Total Number of Experiments</t>
+  </si>
+  <si>
+    <t>DF1 Experiments</t>
+  </si>
+  <si>
+    <t>DF2 Experiments</t>
+  </si>
+  <si>
+    <t>NovelOmics Deep-WES Experiments</t>
+  </si>
+  <si>
+    <t>NovelOmics RNAseq Experiments</t>
+  </si>
+  <si>
+    <t>NovelOmics SR-WGS Experiments</t>
+  </si>
+  <si>
+    <t>NovelOmics WGS Experiments</t>
+  </si>
+  <si>
+    <t>Total Number of Files</t>
+  </si>
+  <si>
+    <t>DF1 Files</t>
+  </si>
+  <si>
+    <t>DF2 Files</t>
+  </si>
+  <si>
+    <t>DF3 Files</t>
+  </si>
+  <si>
+    <t>NovelOmics Deep-WES Files</t>
+  </si>
+  <si>
+    <t>NovelOmics RNAseq Files</t>
+  </si>
+  <si>
+    <t>NovelOmics SR-WGS Files</t>
+  </si>
+  <si>
+    <t>NovelOmics WGS Files</t>
+  </si>
+  <si>
     <t>rd3_sex</t>
   </si>
   <si>
@@ -292,6 +387,9 @@
     <t>rd3_novelrnaseq_sample</t>
   </si>
   <si>
+    <t>rd3_novellrwgs_sample</t>
+  </si>
+  <si>
     <t>rd3_novelsrwgs_sample</t>
   </si>
   <si>
@@ -356,93 +454,6 @@
   </si>
   <si>
     <t>partOfAttribute</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/ExO_0000127</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C142495</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164337</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C80271</t>
-  </si>
-  <si>
-    <t>HL7:C0442737</t>
-  </si>
-  <si>
-    <t>ExO:0000127</t>
-  </si>
-  <si>
-    <t>GSSO:009418</t>
-  </si>
-  <si>
-    <t>NCIT:C142495</t>
-  </si>
-  <si>
-    <t>NCIT:C15607</t>
-  </si>
-  <si>
-    <t>NCIT:C164337</t>
-  </si>
-  <si>
-    <t>NCIT:C16977</t>
-  </si>
-  <si>
-    <t>NCIT:C172217</t>
-  </si>
-  <si>
-    <t>NCIT:C25173</t>
-  </si>
-  <si>
-    <t>NCIT:C64917</t>
-  </si>
-  <si>
-    <t>NCIT:C80271</t>
-  </si>
-  <si>
-    <t>NCIT:C89336</t>
-  </si>
-  <si>
-    <t>RO:0000056</t>
-  </si>
-  <si>
-    <t>HL7</t>
-  </si>
-  <si>
-    <t>ExO</t>
-  </si>
-  <si>
-    <t>GSSO</t>
-  </si>
-  <si>
-    <t>NCIT</t>
-  </si>
-  <si>
-    <t>RO</t>
-  </si>
-  <si>
-    <t>isAssociatedWith</t>
-  </si>
-  <si>
-    <t>http://molgenis.org#isAssociatedWith</t>
-  </si>
-  <si>
-    <t>identifier</t>
-  </si>
-  <si>
-    <t>objectIRI</t>
-  </si>
-  <si>
-    <t>codeSystem</t>
-  </si>
-  <si>
-    <t>relationLabel</t>
-  </si>
-  <si>
-    <t>relationIRI</t>
   </si>
 </sst>
 </file>
@@ -810,13 +821,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>100</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>102</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -845,19 +856,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>136</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>133</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>102</v>
+        <v>135</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>104</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -887,48 +898,51 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>138</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>133</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>102</v>
+        <v>135</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>104</v>
+        <v>137</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>106</v>
+        <v>139</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>107</v>
+        <v>140</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>108</v>
+        <v>141</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>109</v>
+        <v>142</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>110</v>
+        <v>143</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+        <v>144</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -936,13 +950,13 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -957,7 +971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -965,13 +979,13 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -986,10 +1000,13 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>81</v>
+      </c>
+      <c r="K3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -997,13 +1014,13 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -1017,8 +1034,11 @@
       <c r="I4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="J4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1026,13 +1046,13 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -1047,10 +1067,13 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>83</v>
+      </c>
+      <c r="K5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1058,13 +1081,13 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -1079,10 +1102,13 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>84</v>
+      </c>
+      <c r="K6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1090,13 +1116,13 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -1111,10 +1137,13 @@
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>85</v>
+      </c>
+      <c r="K7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1122,10 +1151,10 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -1140,10 +1169,13 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>86</v>
+      </c>
+      <c r="K8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1151,13 +1183,13 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -1172,10 +1204,13 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>15</v>
+      </c>
+      <c r="K9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1183,13 +1218,13 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -1203,8 +1238,11 @@
       <c r="I10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="J10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1212,10 +1250,10 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -1230,7 +1268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1238,13 +1276,13 @@
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
@@ -1258,11 +1296,11 @@
       <c r="I12" t="b">
         <v>0</v>
       </c>
-      <c r="J12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="K12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1270,13 +1308,13 @@
         <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E13" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -1290,11 +1328,11 @@
       <c r="I13" t="b">
         <v>0</v>
       </c>
-      <c r="J13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="K13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1302,13 +1340,13 @@
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -1322,22 +1360,19 @@
       <c r="I14" t="b">
         <v>0</v>
       </c>
-      <c r="J14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="K14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>7</v>
       </c>
       <c r="B15" t="s">
         <v>21</v>
       </c>
-      <c r="C15" t="s">
-        <v>62</v>
-      </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -1352,7 +1387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1360,7 +1395,7 @@
         <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -1374,8 +1409,14 @@
       <c r="I16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="J16" t="s">
+        <v>88</v>
+      </c>
+      <c r="L16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1383,7 +1424,7 @@
         <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
@@ -1397,11 +1438,17 @@
       <c r="I17" t="b">
         <v>0</v>
       </c>
+      <c r="J17" t="s">
+        <v>89</v>
+      </c>
       <c r="K17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+        <v>118</v>
+      </c>
+      <c r="L17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1409,7 +1456,7 @@
         <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
@@ -1424,13 +1471,16 @@
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="K18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+        <v>119</v>
+      </c>
+      <c r="L18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1438,7 +1488,7 @@
         <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -1453,13 +1503,16 @@
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="K19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+        <v>120</v>
+      </c>
+      <c r="L19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1467,7 +1520,7 @@
         <v>26</v>
       </c>
       <c r="E20" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
@@ -1482,13 +1535,16 @@
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="K20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+        <v>121</v>
+      </c>
+      <c r="L20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1496,7 +1552,7 @@
         <v>27</v>
       </c>
       <c r="E21" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
@@ -1511,13 +1567,16 @@
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="K21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+        <v>122</v>
+      </c>
+      <c r="L21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1525,7 +1584,7 @@
         <v>28</v>
       </c>
       <c r="E22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
@@ -1540,13 +1599,16 @@
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="K22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+        <v>123</v>
+      </c>
+      <c r="L22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1554,7 +1616,7 @@
         <v>29</v>
       </c>
       <c r="E23" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -1569,13 +1631,16 @@
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="K23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+        <v>124</v>
+      </c>
+      <c r="L23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1583,7 +1648,7 @@
         <v>30</v>
       </c>
       <c r="E24" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
@@ -1598,13 +1663,16 @@
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="K24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+        <v>125</v>
+      </c>
+      <c r="L24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -1612,7 +1680,7 @@
         <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
@@ -1627,7 +1695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1635,7 +1703,7 @@
         <v>32</v>
       </c>
       <c r="E26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
@@ -1649,11 +1717,14 @@
       <c r="I26" t="b">
         <v>0</v>
       </c>
-      <c r="K26" t="s">
+      <c r="J26" t="s">
+        <v>97</v>
+      </c>
+      <c r="L26" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1661,7 +1732,7 @@
         <v>33</v>
       </c>
       <c r="E27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
@@ -1676,13 +1747,16 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="K27" t="s">
+        <v>126</v>
+      </c>
+      <c r="L27" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1690,7 +1764,7 @@
         <v>34</v>
       </c>
       <c r="E28" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F28" t="b">
         <v>0</v>
@@ -1705,13 +1779,16 @@
         <v>0</v>
       </c>
       <c r="J28" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="K28" t="s">
+        <v>127</v>
+      </c>
+      <c r="L28" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1719,7 +1796,7 @@
         <v>35</v>
       </c>
       <c r="E29" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F29" t="b">
         <v>0</v>
@@ -1734,13 +1811,16 @@
         <v>0</v>
       </c>
       <c r="J29" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="K29" t="s">
+        <v>128</v>
+      </c>
+      <c r="L29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -1748,7 +1828,7 @@
         <v>36</v>
       </c>
       <c r="E30" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F30" t="b">
         <v>0</v>
@@ -1763,13 +1843,16 @@
         <v>0</v>
       </c>
       <c r="J30" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="K30" t="s">
+        <v>129</v>
+      </c>
+      <c r="L30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1777,7 +1860,7 @@
         <v>37</v>
       </c>
       <c r="E31" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
@@ -1792,13 +1875,16 @@
         <v>0</v>
       </c>
       <c r="J31" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="K31" t="s">
+        <v>130</v>
+      </c>
+      <c r="L31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1806,7 +1892,7 @@
         <v>38</v>
       </c>
       <c r="E32" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F32" t="b">
         <v>0</v>
@@ -1821,13 +1907,16 @@
         <v>0</v>
       </c>
       <c r="J32" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="K32" t="s">
+        <v>131</v>
+      </c>
+      <c r="L32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -1835,7 +1924,7 @@
         <v>39</v>
       </c>
       <c r="E33" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F33" t="b">
         <v>0</v>
@@ -1850,13 +1939,16 @@
         <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="K33" t="s">
+        <v>132</v>
+      </c>
+      <c r="L33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -1864,7 +1956,7 @@
         <v>40</v>
       </c>
       <c r="E34" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
@@ -1879,7 +1971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -1887,7 +1979,7 @@
         <v>41</v>
       </c>
       <c r="E35" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
@@ -1901,11 +1993,14 @@
       <c r="I35" t="b">
         <v>0</v>
       </c>
-      <c r="K35" t="s">
+      <c r="J35" t="s">
+        <v>104</v>
+      </c>
+      <c r="L35" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -1913,7 +2008,7 @@
         <v>42</v>
       </c>
       <c r="E36" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
@@ -1927,11 +2022,14 @@
       <c r="I36" t="b">
         <v>0</v>
       </c>
-      <c r="K36" t="s">
+      <c r="J36" t="s">
+        <v>105</v>
+      </c>
+      <c r="L36" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1939,7 +2037,7 @@
         <v>43</v>
       </c>
       <c r="E37" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F37" t="b">
         <v>0</v>
@@ -1953,11 +2051,14 @@
       <c r="I37" t="b">
         <v>0</v>
       </c>
-      <c r="K37" t="s">
+      <c r="J37" t="s">
+        <v>106</v>
+      </c>
+      <c r="L37" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:12">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -1965,7 +2066,7 @@
         <v>44</v>
       </c>
       <c r="E38" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F38" t="b">
         <v>0</v>
@@ -1979,11 +2080,14 @@
       <c r="I38" t="b">
         <v>0</v>
       </c>
-      <c r="K38" t="s">
+      <c r="J38" t="s">
+        <v>107</v>
+      </c>
+      <c r="L38" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:12">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1991,7 +2095,7 @@
         <v>45</v>
       </c>
       <c r="E39" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
@@ -2005,11 +2109,14 @@
       <c r="I39" t="b">
         <v>0</v>
       </c>
-      <c r="K39" t="s">
+      <c r="J39" t="s">
+        <v>108</v>
+      </c>
+      <c r="L39" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:12">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -2017,7 +2124,7 @@
         <v>46</v>
       </c>
       <c r="E40" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F40" t="b">
         <v>0</v>
@@ -2031,11 +2138,14 @@
       <c r="I40" t="b">
         <v>0</v>
       </c>
-      <c r="K40" t="s">
+      <c r="J40" t="s">
+        <v>109</v>
+      </c>
+      <c r="L40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:12">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -2043,7 +2153,7 @@
         <v>47</v>
       </c>
       <c r="E41" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F41" t="b">
         <v>0</v>
@@ -2057,11 +2167,14 @@
       <c r="I41" t="b">
         <v>0</v>
       </c>
-      <c r="K41" t="s">
+      <c r="J41" t="s">
+        <v>110</v>
+      </c>
+      <c r="L41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:12">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -2069,7 +2182,7 @@
         <v>48</v>
       </c>
       <c r="E42" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F42" t="b">
         <v>0</v>
@@ -2083,8 +2196,37 @@
       <c r="I42" t="b">
         <v>0</v>
       </c>
-      <c r="K42" t="s">
+      <c r="J42" t="s">
+        <v>111</v>
+      </c>
+      <c r="L42" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" t="s">
+        <v>63</v>
+      </c>
+      <c r="E43" t="s">
+        <v>74</v>
+      </c>
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+      <c r="G43" t="b">
+        <v>0</v>
+      </c>
+      <c r="H43" t="b">
+        <v>1</v>
+      </c>
+      <c r="I43" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2103,338 +2245,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E3" t="s">
-        <v>135</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E4" t="s">
-        <v>135</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" t="s">
-        <v>133</v>
-      </c>
-      <c r="E5" t="s">
-        <v>135</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" t="s">
-        <v>133</v>
-      </c>
-      <c r="E6" t="s">
-        <v>135</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" t="s">
-        <v>122</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D7" t="s">
-        <v>133</v>
-      </c>
-      <c r="E7" t="s">
-        <v>135</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" t="s">
-        <v>123</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" t="s">
-        <v>133</v>
-      </c>
-      <c r="E8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" t="s">
-        <v>133</v>
-      </c>
-      <c r="E9" t="s">
-        <v>135</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" t="s">
-        <v>125</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" t="s">
-        <v>133</v>
-      </c>
-      <c r="E10" t="s">
-        <v>135</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" t="s">
-        <v>126</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" t="s">
-        <v>133</v>
-      </c>
-      <c r="E11" t="s">
-        <v>135</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B12" t="s">
-        <v>127</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D12" t="s">
-        <v>133</v>
-      </c>
-      <c r="E12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" t="s">
-        <v>128</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" t="s">
-        <v>133</v>
-      </c>
-      <c r="E13" t="s">
-        <v>135</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" t="s">
-        <v>129</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" t="s">
-        <v>134</v>
-      </c>
-      <c r="E14" t="s">
-        <v>135</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="F2" r:id="rId3" location="isAssociatedWith"/>
-    <hyperlink ref="A3" r:id="rId4"/>
-    <hyperlink ref="C3" r:id="rId5"/>
-    <hyperlink ref="F3" r:id="rId6" location="isAssociatedWith"/>
-    <hyperlink ref="A4" r:id="rId7"/>
-    <hyperlink ref="C4" r:id="rId8"/>
-    <hyperlink ref="F4" r:id="rId9" location="isAssociatedWith"/>
-    <hyperlink ref="A5" r:id="rId10"/>
-    <hyperlink ref="C5" r:id="rId11"/>
-    <hyperlink ref="F5" r:id="rId12" location="isAssociatedWith"/>
-    <hyperlink ref="A6" r:id="rId13"/>
-    <hyperlink ref="C6" r:id="rId14"/>
-    <hyperlink ref="F6" r:id="rId15" location="isAssociatedWith"/>
-    <hyperlink ref="A7" r:id="rId16"/>
-    <hyperlink ref="C7" r:id="rId17"/>
-    <hyperlink ref="F7" r:id="rId18" location="isAssociatedWith"/>
-    <hyperlink ref="A8" r:id="rId19"/>
-    <hyperlink ref="C8" r:id="rId20"/>
-    <hyperlink ref="F8" r:id="rId21" location="isAssociatedWith"/>
-    <hyperlink ref="A9" r:id="rId22"/>
-    <hyperlink ref="C9" r:id="rId23"/>
-    <hyperlink ref="F9" r:id="rId24" location="isAssociatedWith"/>
-    <hyperlink ref="A10" r:id="rId25"/>
-    <hyperlink ref="C10" r:id="rId26"/>
-    <hyperlink ref="F10" r:id="rId27" location="isAssociatedWith"/>
-    <hyperlink ref="A11" r:id="rId28"/>
-    <hyperlink ref="C11" r:id="rId29"/>
-    <hyperlink ref="F11" r:id="rId30" location="isAssociatedWith"/>
-    <hyperlink ref="A12" r:id="rId31"/>
-    <hyperlink ref="C12" r:id="rId32"/>
-    <hyperlink ref="F12" r:id="rId33" location="isAssociatedWith"/>
-    <hyperlink ref="A13" r:id="rId34"/>
-    <hyperlink ref="C13" r:id="rId35"/>
-    <hyperlink ref="F13" r:id="rId36" location="isAssociatedWith"/>
-    <hyperlink ref="A14" r:id="rId37"/>
-    <hyperlink ref="C14" r:id="rId38"/>
-    <hyperlink ref="F14" r:id="rId39" location="isAssociatedWith"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added column to group subjects with certain types of data
</commit_message>
<xml_diff>
--- a/dist/rd3_overview.xlsx
+++ b/dist/rd3_overview.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="148">
   <si>
     <t>rd3</t>
   </si>
@@ -60,6 +60,9 @@
     <t>patch</t>
   </si>
   <si>
+    <t>hasOnlyNovelOmics</t>
+  </si>
+  <si>
     <t>organisation</t>
   </si>
   <si>
@@ -184,6 +187,9 @@
   </si>
   <si>
     <t>The act of making data or other structured information accessible to the public or to the user group of a database.</t>
+  </si>
+  <si>
+    <t>If true, this subject does not have data in any data freeze (1,2,3,etc.)</t>
   </si>
   <si>
     <t>The most significant institute for medical consultation and/or study inclusion in context of the genetic disease of this person.</t>
@@ -821,13 +827,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -856,19 +862,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -898,7 +904,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -906,40 +912,40 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -950,13 +956,13 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -979,13 +985,13 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -1000,10 +1006,10 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1014,13 +1020,13 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -1035,7 +1041,7 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1046,13 +1052,13 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -1067,7 +1073,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K5" t="s">
         <v>7</v>
@@ -1081,13 +1087,13 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -1102,7 +1108,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="K6" t="s">
         <v>7</v>
@@ -1116,13 +1122,13 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -1137,10 +1143,10 @@
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="K7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1151,10 +1157,10 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -1167,12 +1173,6 @@
       </c>
       <c r="I8" t="b">
         <v>0</v>
-      </c>
-      <c r="J8" t="s">
-        <v>86</v>
-      </c>
-      <c r="K8" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1183,13 +1183,10 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -1204,10 +1201,10 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
       <c r="K9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1218,10 +1215,10 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
         <v>77</v>
@@ -1239,7 +1236,10 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>87</v>
+        <v>16</v>
+      </c>
+      <c r="K10" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1250,10 +1250,13 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="E11" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -1266,6 +1269,9 @@
       </c>
       <c r="I11" t="b">
         <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1276,13 +1282,10 @@
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
@@ -1295,9 +1298,6 @@
       </c>
       <c r="I12" t="b">
         <v>0</v>
-      </c>
-      <c r="K12" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1308,13 +1308,13 @@
         <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -1329,7 +1329,7 @@
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1340,13 +1340,13 @@
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E14" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -1361,7 +1361,7 @@
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1371,8 +1371,14 @@
       <c r="B15" t="s">
         <v>21</v>
       </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -1385,6 +1391,9 @@
       </c>
       <c r="I15" t="b">
         <v>0</v>
+      </c>
+      <c r="K15" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1395,7 +1404,7 @@
         <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -1408,12 +1417,6 @@
       </c>
       <c r="I16" t="b">
         <v>0</v>
-      </c>
-      <c r="J16" t="s">
-        <v>88</v>
-      </c>
-      <c r="L16" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1424,7 +1427,7 @@
         <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
@@ -1439,13 +1442,10 @@
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>89</v>
-      </c>
-      <c r="K17" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="L17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1456,7 +1456,7 @@
         <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
@@ -1471,13 +1471,13 @@
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="L18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1488,7 +1488,7 @@
         <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -1503,13 +1503,13 @@
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K19" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1520,7 +1520,7 @@
         <v>26</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
@@ -1535,13 +1535,13 @@
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K20" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1552,7 +1552,7 @@
         <v>27</v>
       </c>
       <c r="E21" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
@@ -1567,13 +1567,13 @@
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K21" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="L21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1584,7 +1584,7 @@
         <v>28</v>
       </c>
       <c r="E22" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
@@ -1599,13 +1599,13 @@
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K22" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1616,7 +1616,7 @@
         <v>29</v>
       </c>
       <c r="E23" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -1631,13 +1631,13 @@
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="L23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1648,7 +1648,7 @@
         <v>30</v>
       </c>
       <c r="E24" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
@@ -1663,13 +1663,13 @@
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K24" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1680,7 +1680,7 @@
         <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
@@ -1693,6 +1693,15 @@
       </c>
       <c r="I25" t="b">
         <v>0</v>
+      </c>
+      <c r="J25" t="s">
+        <v>98</v>
+      </c>
+      <c r="K25" t="s">
+        <v>127</v>
+      </c>
+      <c r="L25" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1703,7 +1712,7 @@
         <v>32</v>
       </c>
       <c r="E26" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
@@ -1716,12 +1725,6 @@
       </c>
       <c r="I26" t="b">
         <v>0</v>
-      </c>
-      <c r="J26" t="s">
-        <v>97</v>
-      </c>
-      <c r="L26" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1732,7 +1735,7 @@
         <v>33</v>
       </c>
       <c r="E27" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
@@ -1747,13 +1750,10 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>98</v>
-      </c>
-      <c r="K27" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="L27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1764,7 +1764,7 @@
         <v>34</v>
       </c>
       <c r="E28" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F28" t="b">
         <v>0</v>
@@ -1779,13 +1779,13 @@
         <v>0</v>
       </c>
       <c r="J28" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K28" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="L28" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1796,7 +1796,7 @@
         <v>35</v>
       </c>
       <c r="E29" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F29" t="b">
         <v>0</v>
@@ -1811,13 +1811,13 @@
         <v>0</v>
       </c>
       <c r="J29" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="K29" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="L29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1828,7 +1828,7 @@
         <v>36</v>
       </c>
       <c r="E30" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F30" t="b">
         <v>0</v>
@@ -1846,10 +1846,10 @@
         <v>100</v>
       </c>
       <c r="K30" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="L30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1860,7 +1860,7 @@
         <v>37</v>
       </c>
       <c r="E31" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
@@ -1875,13 +1875,13 @@
         <v>0</v>
       </c>
       <c r="J31" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K31" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="L31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -1892,7 +1892,7 @@
         <v>38</v>
       </c>
       <c r="E32" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F32" t="b">
         <v>0</v>
@@ -1907,13 +1907,13 @@
         <v>0</v>
       </c>
       <c r="J32" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K32" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -1924,7 +1924,7 @@
         <v>39</v>
       </c>
       <c r="E33" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F33" t="b">
         <v>0</v>
@@ -1939,13 +1939,13 @@
         <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="K33" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="L33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -1956,7 +1956,7 @@
         <v>40</v>
       </c>
       <c r="E34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
@@ -1969,6 +1969,15 @@
       </c>
       <c r="I34" t="b">
         <v>0</v>
+      </c>
+      <c r="J34" t="s">
+        <v>105</v>
+      </c>
+      <c r="K34" t="s">
+        <v>134</v>
+      </c>
+      <c r="L34" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -1979,7 +1988,7 @@
         <v>41</v>
       </c>
       <c r="E35" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
@@ -1992,12 +2001,6 @@
       </c>
       <c r="I35" t="b">
         <v>0</v>
-      </c>
-      <c r="J35" t="s">
-        <v>104</v>
-      </c>
-      <c r="L35" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -2008,7 +2011,7 @@
         <v>42</v>
       </c>
       <c r="E36" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
@@ -2023,10 +2026,10 @@
         <v>0</v>
       </c>
       <c r="J36" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="L36" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -2037,7 +2040,7 @@
         <v>43</v>
       </c>
       <c r="E37" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F37" t="b">
         <v>0</v>
@@ -2052,10 +2055,10 @@
         <v>0</v>
       </c>
       <c r="J37" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="L37" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -2066,7 +2069,7 @@
         <v>44</v>
       </c>
       <c r="E38" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F38" t="b">
         <v>0</v>
@@ -2081,10 +2084,10 @@
         <v>0</v>
       </c>
       <c r="J38" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L38" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2095,7 +2098,7 @@
         <v>45</v>
       </c>
       <c r="E39" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
@@ -2110,10 +2113,10 @@
         <v>0</v>
       </c>
       <c r="J39" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L39" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2124,7 +2127,7 @@
         <v>46</v>
       </c>
       <c r="E40" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F40" t="b">
         <v>0</v>
@@ -2139,10 +2142,10 @@
         <v>0</v>
       </c>
       <c r="J40" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="L40" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2153,7 +2156,7 @@
         <v>47</v>
       </c>
       <c r="E41" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F41" t="b">
         <v>0</v>
@@ -2168,10 +2171,10 @@
         <v>0</v>
       </c>
       <c r="J41" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L41" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2182,7 +2185,7 @@
         <v>48</v>
       </c>
       <c r="E42" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F42" t="b">
         <v>0</v>
@@ -2197,10 +2200,10 @@
         <v>0</v>
       </c>
       <c r="J42" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="L42" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -2210,11 +2213,8 @@
       <c r="B43" t="s">
         <v>49</v>
       </c>
-      <c r="C43" t="s">
-        <v>63</v>
-      </c>
       <c r="E43" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F43" t="b">
         <v>0</v>
@@ -2226,6 +2226,38 @@
         <v>1</v>
       </c>
       <c r="I43" t="b">
+        <v>0</v>
+      </c>
+      <c r="J43" t="s">
+        <v>113</v>
+      </c>
+      <c r="L43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" t="s">
+        <v>65</v>
+      </c>
+      <c r="E44" t="s">
+        <v>76</v>
+      </c>
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44" t="b">
+        <v>0</v>
+      </c>
+      <c r="H44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2237,11 +2269,11 @@
     <hyperlink ref="D5" r:id="rId4"/>
     <hyperlink ref="D6" r:id="rId5"/>
     <hyperlink ref="D7" r:id="rId6"/>
-    <hyperlink ref="D9" r:id="rId7"/>
-    <hyperlink ref="D10" r:id="rId8"/>
-    <hyperlink ref="D12" r:id="rId9"/>
-    <hyperlink ref="D13" r:id="rId10"/>
-    <hyperlink ref="D14" r:id="rId11"/>
+    <hyperlink ref="D10" r:id="rId7"/>
+    <hyperlink ref="D11" r:id="rId8"/>
+    <hyperlink ref="D13" r:id="rId9"/>
+    <hyperlink ref="D14" r:id="rId10"/>
+    <hyperlink ref="D15" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added missing tags component
</commit_message>
<xml_diff>
--- a/dist/rd3_overview.xlsx
+++ b/dist/rd3_overview.xlsx
@@ -10,13 +10,14 @@
     <sheet name="packages" sheetId="1" r:id="rId1"/>
     <sheet name="entities" sheetId="2" r:id="rId2"/>
     <sheet name="attributes" sheetId="3" r:id="rId3"/>
+    <sheet name="tags" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="177">
   <si>
     <t>rd3</t>
   </si>
@@ -460,6 +461,93 @@
   </si>
   <si>
     <t>partOfAttribute</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ExO_0000127</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C142495</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164337</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C80271</t>
+  </si>
+  <si>
+    <t>HL7:C0442737</t>
+  </si>
+  <si>
+    <t>ExO:0000127</t>
+  </si>
+  <si>
+    <t>GSSO:009418</t>
+  </si>
+  <si>
+    <t>NCIT:C142495</t>
+  </si>
+  <si>
+    <t>NCIT:C15607</t>
+  </si>
+  <si>
+    <t>NCIT:C164337</t>
+  </si>
+  <si>
+    <t>NCIT:C16977</t>
+  </si>
+  <si>
+    <t>NCIT:C172217</t>
+  </si>
+  <si>
+    <t>NCIT:C25173</t>
+  </si>
+  <si>
+    <t>NCIT:C64917</t>
+  </si>
+  <si>
+    <t>NCIT:C80271</t>
+  </si>
+  <si>
+    <t>NCIT:C89336</t>
+  </si>
+  <si>
+    <t>RO:0000056</t>
+  </si>
+  <si>
+    <t>HL7</t>
+  </si>
+  <si>
+    <t>ExO</t>
+  </si>
+  <si>
+    <t>GSSO</t>
+  </si>
+  <si>
+    <t>NCIT</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>isAssociatedWith</t>
+  </si>
+  <si>
+    <t>http://molgenis.org#isAssociatedWith</t>
+  </si>
+  <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>objectIRI</t>
+  </si>
+  <si>
+    <t>codeSystem</t>
+  </si>
+  <si>
+    <t>relationLabel</t>
+  </si>
+  <si>
+    <t>relationIRI</t>
   </si>
 </sst>
 </file>
@@ -2277,4 +2365,338 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E6" t="s">
+        <v>170</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E7" t="s">
+        <v>170</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" t="s">
+        <v>168</v>
+      </c>
+      <c r="E8" t="s">
+        <v>170</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E9" t="s">
+        <v>170</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E10" t="s">
+        <v>170</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" t="s">
+        <v>168</v>
+      </c>
+      <c r="E11" t="s">
+        <v>170</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D12" t="s">
+        <v>168</v>
+      </c>
+      <c r="E12" t="s">
+        <v>170</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" t="s">
+        <v>168</v>
+      </c>
+      <c r="E13" t="s">
+        <v>170</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
+        <v>164</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" t="s">
+        <v>169</v>
+      </c>
+      <c r="E14" t="s">
+        <v>170</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="F2" r:id="rId3" location="isAssociatedWith"/>
+    <hyperlink ref="A3" r:id="rId4"/>
+    <hyperlink ref="C3" r:id="rId5"/>
+    <hyperlink ref="F3" r:id="rId6" location="isAssociatedWith"/>
+    <hyperlink ref="A4" r:id="rId7"/>
+    <hyperlink ref="C4" r:id="rId8"/>
+    <hyperlink ref="F4" r:id="rId9" location="isAssociatedWith"/>
+    <hyperlink ref="A5" r:id="rId10"/>
+    <hyperlink ref="C5" r:id="rId11"/>
+    <hyperlink ref="F5" r:id="rId12" location="isAssociatedWith"/>
+    <hyperlink ref="A6" r:id="rId13"/>
+    <hyperlink ref="C6" r:id="rId14"/>
+    <hyperlink ref="F6" r:id="rId15" location="isAssociatedWith"/>
+    <hyperlink ref="A7" r:id="rId16"/>
+    <hyperlink ref="C7" r:id="rId17"/>
+    <hyperlink ref="F7" r:id="rId18" location="isAssociatedWith"/>
+    <hyperlink ref="A8" r:id="rId19"/>
+    <hyperlink ref="C8" r:id="rId20"/>
+    <hyperlink ref="F8" r:id="rId21" location="isAssociatedWith"/>
+    <hyperlink ref="A9" r:id="rId22"/>
+    <hyperlink ref="C9" r:id="rId23"/>
+    <hyperlink ref="F9" r:id="rId24" location="isAssociatedWith"/>
+    <hyperlink ref="A10" r:id="rId25"/>
+    <hyperlink ref="C10" r:id="rId26"/>
+    <hyperlink ref="F10" r:id="rId27" location="isAssociatedWith"/>
+    <hyperlink ref="A11" r:id="rId28"/>
+    <hyperlink ref="C11" r:id="rId29"/>
+    <hyperlink ref="F11" r:id="rId30" location="isAssociatedWith"/>
+    <hyperlink ref="A12" r:id="rId31"/>
+    <hyperlink ref="C12" r:id="rId32"/>
+    <hyperlink ref="F12" r:id="rId33" location="isAssociatedWith"/>
+    <hyperlink ref="A13" r:id="rId34"/>
+    <hyperlink ref="C13" r:id="rId35"/>
+    <hyperlink ref="F13" r:id="rId36" location="isAssociatedWith"/>
+    <hyperlink ref="A14" r:id="rId37"/>
+    <hyperlink ref="C14" r:id="rId38"/>
+    <hyperlink ref="F14" r:id="rId39" location="isAssociatedWith"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
minor changes to view emx
</commit_message>
<xml_diff>
--- a/dist/rd3_overview.xlsx
+++ b/dist/rd3_overview.xlsx
@@ -10,14 +10,13 @@
     <sheet name="packages" sheetId="1" r:id="rId1"/>
     <sheet name="entities" sheetId="2" r:id="rId2"/>
     <sheet name="attributes" sheetId="3" r:id="rId3"/>
-    <sheet name="tags" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="147">
   <si>
     <t>rd3</t>
   </si>
@@ -169,7 +168,7 @@
     <t>novelwgsFiles</t>
   </si>
   <si>
-    <t>associatedRD3Releases</t>
+    <t>emxReleases</t>
   </si>
   <si>
     <t>A unique proper name or character sequence that identifies this particular individual who is the subject of personal data, persons to whom data refers, and from whom data are collected, processed, and stored.</t>
@@ -253,9 +252,6 @@
     <t>mref</t>
   </si>
   <si>
-    <t>xref</t>
-  </si>
-  <si>
     <t>bool</t>
   </si>
   <si>
@@ -461,93 +457,6 @@
   </si>
   <si>
     <t>partOfAttribute</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/ExO_0000127</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C142495</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164337</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C80271</t>
-  </si>
-  <si>
-    <t>HL7:C0442737</t>
-  </si>
-  <si>
-    <t>ExO:0000127</t>
-  </si>
-  <si>
-    <t>GSSO:009418</t>
-  </si>
-  <si>
-    <t>NCIT:C142495</t>
-  </si>
-  <si>
-    <t>NCIT:C15607</t>
-  </si>
-  <si>
-    <t>NCIT:C164337</t>
-  </si>
-  <si>
-    <t>NCIT:C16977</t>
-  </si>
-  <si>
-    <t>NCIT:C172217</t>
-  </si>
-  <si>
-    <t>NCIT:C25173</t>
-  </si>
-  <si>
-    <t>NCIT:C64917</t>
-  </si>
-  <si>
-    <t>NCIT:C80271</t>
-  </si>
-  <si>
-    <t>NCIT:C89336</t>
-  </si>
-  <si>
-    <t>RO:0000056</t>
-  </si>
-  <si>
-    <t>HL7</t>
-  </si>
-  <si>
-    <t>ExO</t>
-  </si>
-  <si>
-    <t>GSSO</t>
-  </si>
-  <si>
-    <t>NCIT</t>
-  </si>
-  <si>
-    <t>RO</t>
-  </si>
-  <si>
-    <t>isAssociatedWith</t>
-  </si>
-  <si>
-    <t>http://molgenis.org#isAssociatedWith</t>
-  </si>
-  <si>
-    <t>identifier</t>
-  </si>
-  <si>
-    <t>objectIRI</t>
-  </si>
-  <si>
-    <t>codeSystem</t>
-  </si>
-  <si>
-    <t>relationLabel</t>
-  </si>
-  <si>
-    <t>relationIRI</t>
   </si>
 </sst>
 </file>
@@ -915,13 +824,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -950,19 +859,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1000,40 +909,40 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1094,10 +1003,10 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1129,7 +1038,7 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1146,7 +1055,7 @@
         <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -1161,7 +1070,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K5" t="s">
         <v>7</v>
@@ -1181,7 +1090,7 @@
         <v>69</v>
       </c>
       <c r="E6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -1196,7 +1105,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K6" t="s">
         <v>7</v>
@@ -1231,10 +1140,10 @@
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1248,7 +1157,7 @@
         <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -1289,10 +1198,10 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1327,7 +1236,7 @@
         <v>16</v>
       </c>
       <c r="K10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1344,7 +1253,7 @@
         <v>72</v>
       </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -1359,7 +1268,7 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1373,7 +1282,7 @@
         <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
@@ -1417,7 +1326,7 @@
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1449,7 +1358,7 @@
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1481,7 +1390,7 @@
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1492,7 +1401,7 @@
         <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -1515,7 +1424,7 @@
         <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
@@ -1530,7 +1439,7 @@
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L17" t="s">
         <v>22</v>
@@ -1559,10 +1468,10 @@
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L18" t="s">
         <v>22</v>
@@ -1591,10 +1500,10 @@
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L19" t="s">
         <v>22</v>
@@ -1623,10 +1532,10 @@
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L20" t="s">
         <v>22</v>
@@ -1655,10 +1564,10 @@
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L21" t="s">
         <v>22</v>
@@ -1687,10 +1596,10 @@
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L22" t="s">
         <v>22</v>
@@ -1719,10 +1628,10 @@
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L23" t="s">
         <v>22</v>
@@ -1751,10 +1660,10 @@
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L24" t="s">
         <v>22</v>
@@ -1783,10 +1692,10 @@
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L25" t="s">
         <v>22</v>
@@ -1800,7 +1709,7 @@
         <v>32</v>
       </c>
       <c r="E26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
@@ -1823,7 +1732,7 @@
         <v>33</v>
       </c>
       <c r="E27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
@@ -1838,7 +1747,7 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L27" t="s">
         <v>32</v>
@@ -1867,10 +1776,10 @@
         <v>0</v>
       </c>
       <c r="J28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L28" t="s">
         <v>32</v>
@@ -1899,10 +1808,10 @@
         <v>0</v>
       </c>
       <c r="J29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L29" t="s">
         <v>32</v>
@@ -1931,10 +1840,10 @@
         <v>0</v>
       </c>
       <c r="J30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L30" t="s">
         <v>32</v>
@@ -1963,10 +1872,10 @@
         <v>0</v>
       </c>
       <c r="J31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L31" t="s">
         <v>32</v>
@@ -1995,10 +1904,10 @@
         <v>0</v>
       </c>
       <c r="J32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L32" t="s">
         <v>32</v>
@@ -2027,10 +1936,10 @@
         <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L33" t="s">
         <v>32</v>
@@ -2059,10 +1968,10 @@
         <v>0</v>
       </c>
       <c r="J34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L34" t="s">
         <v>32</v>
@@ -2076,7 +1985,7 @@
         <v>41</v>
       </c>
       <c r="E35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
@@ -2099,7 +2008,7 @@
         <v>42</v>
       </c>
       <c r="E36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
@@ -2114,7 +2023,7 @@
         <v>0</v>
       </c>
       <c r="J36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L36" t="s">
         <v>41</v>
@@ -2128,7 +2037,7 @@
         <v>43</v>
       </c>
       <c r="E37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F37" t="b">
         <v>0</v>
@@ -2143,7 +2052,7 @@
         <v>0</v>
       </c>
       <c r="J37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L37" t="s">
         <v>41</v>
@@ -2157,7 +2066,7 @@
         <v>44</v>
       </c>
       <c r="E38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F38" t="b">
         <v>0</v>
@@ -2172,7 +2081,7 @@
         <v>0</v>
       </c>
       <c r="J38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L38" t="s">
         <v>41</v>
@@ -2186,7 +2095,7 @@
         <v>45</v>
       </c>
       <c r="E39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
@@ -2201,7 +2110,7 @@
         <v>0</v>
       </c>
       <c r="J39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L39" t="s">
         <v>41</v>
@@ -2215,7 +2124,7 @@
         <v>46</v>
       </c>
       <c r="E40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F40" t="b">
         <v>0</v>
@@ -2230,7 +2139,7 @@
         <v>0</v>
       </c>
       <c r="J40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L40" t="s">
         <v>41</v>
@@ -2244,7 +2153,7 @@
         <v>47</v>
       </c>
       <c r="E41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F41" t="b">
         <v>0</v>
@@ -2259,7 +2168,7 @@
         <v>0</v>
       </c>
       <c r="J41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L41" t="s">
         <v>41</v>
@@ -2273,7 +2182,7 @@
         <v>48</v>
       </c>
       <c r="E42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F42" t="b">
         <v>0</v>
@@ -2288,7 +2197,7 @@
         <v>0</v>
       </c>
       <c r="J42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L42" t="s">
         <v>41</v>
@@ -2302,7 +2211,7 @@
         <v>49</v>
       </c>
       <c r="E43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F43" t="b">
         <v>0</v>
@@ -2317,7 +2226,7 @@
         <v>0</v>
       </c>
       <c r="J43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L43" t="s">
         <v>41</v>
@@ -2365,338 +2274,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D3" t="s">
-        <v>166</v>
-      </c>
-      <c r="E3" t="s">
-        <v>170</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" t="s">
-        <v>167</v>
-      </c>
-      <c r="E4" t="s">
-        <v>170</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E5" t="s">
-        <v>170</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" t="s">
-        <v>156</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E6" t="s">
-        <v>170</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B7" t="s">
-        <v>157</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D7" t="s">
-        <v>168</v>
-      </c>
-      <c r="E7" t="s">
-        <v>170</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" t="s">
-        <v>158</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" t="s">
-        <v>168</v>
-      </c>
-      <c r="E8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" t="s">
-        <v>159</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" t="s">
-        <v>168</v>
-      </c>
-      <c r="E9" t="s">
-        <v>170</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" t="s">
-        <v>160</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" t="s">
-        <v>168</v>
-      </c>
-      <c r="E10" t="s">
-        <v>170</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11" t="s">
-        <v>161</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" t="s">
-        <v>168</v>
-      </c>
-      <c r="E11" t="s">
-        <v>170</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B12" t="s">
-        <v>162</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D12" t="s">
-        <v>168</v>
-      </c>
-      <c r="E12" t="s">
-        <v>170</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" t="s">
-        <v>163</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" t="s">
-        <v>168</v>
-      </c>
-      <c r="E13" t="s">
-        <v>170</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" t="s">
-        <v>164</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" t="s">
-        <v>169</v>
-      </c>
-      <c r="E14" t="s">
-        <v>170</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="F2" r:id="rId3" location="isAssociatedWith"/>
-    <hyperlink ref="A3" r:id="rId4"/>
-    <hyperlink ref="C3" r:id="rId5"/>
-    <hyperlink ref="F3" r:id="rId6" location="isAssociatedWith"/>
-    <hyperlink ref="A4" r:id="rId7"/>
-    <hyperlink ref="C4" r:id="rId8"/>
-    <hyperlink ref="F4" r:id="rId9" location="isAssociatedWith"/>
-    <hyperlink ref="A5" r:id="rId10"/>
-    <hyperlink ref="C5" r:id="rId11"/>
-    <hyperlink ref="F5" r:id="rId12" location="isAssociatedWith"/>
-    <hyperlink ref="A6" r:id="rId13"/>
-    <hyperlink ref="C6" r:id="rId14"/>
-    <hyperlink ref="F6" r:id="rId15" location="isAssociatedWith"/>
-    <hyperlink ref="A7" r:id="rId16"/>
-    <hyperlink ref="C7" r:id="rId17"/>
-    <hyperlink ref="F7" r:id="rId18" location="isAssociatedWith"/>
-    <hyperlink ref="A8" r:id="rId19"/>
-    <hyperlink ref="C8" r:id="rId20"/>
-    <hyperlink ref="F8" r:id="rId21" location="isAssociatedWith"/>
-    <hyperlink ref="A9" r:id="rId22"/>
-    <hyperlink ref="C9" r:id="rId23"/>
-    <hyperlink ref="F9" r:id="rId24" location="isAssociatedWith"/>
-    <hyperlink ref="A10" r:id="rId25"/>
-    <hyperlink ref="C10" r:id="rId26"/>
-    <hyperlink ref="F10" r:id="rId27" location="isAssociatedWith"/>
-    <hyperlink ref="A11" r:id="rId28"/>
-    <hyperlink ref="C11" r:id="rId29"/>
-    <hyperlink ref="F11" r:id="rId30" location="isAssociatedWith"/>
-    <hyperlink ref="A12" r:id="rId31"/>
-    <hyperlink ref="C12" r:id="rId32"/>
-    <hyperlink ref="F12" r:id="rId33" location="isAssociatedWith"/>
-    <hyperlink ref="A13" r:id="rId34"/>
-    <hyperlink ref="C13" r:id="rId35"/>
-    <hyperlink ref="F13" r:id="rId36" location="isAssociatedWith"/>
-    <hyperlink ref="A14" r:id="rId37"/>
-    <hyperlink ref="C14" r:id="rId38"/>
-    <hyperlink ref="F14" r:id="rId39" location="isAssociatedWith"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>